<commit_message>
More 2024AA releasedoc license script updates
</commit_message>
<xml_diff>
--- a/umls.nlm.nih.gov/releasedocs/2024AA/Scripts/Copyright script/requirements/Requirements/All release tasks2.xlsx
+++ b/umls.nlm.nih.gov/releasedocs/2024AA/Scripts/Copyright script/requirements/Requirements/All release tasks2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\SHARE\Rewolinski\Automating release files\Scripts\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rewolinskija\Documents\umls-source-release\umls.nlm.nih.gov\releasedocs\2024AA\Scripts\Copyright script\requirements\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F94D8B-70B4-4DF0-B684-BCF66370AE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3545312-24F1-4451-B5D4-96EC0D45F9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B1BF124-1C1D-4D79-8611-A38D32B5BCD6}"/>
   </bookViews>
@@ -2940,7 +2940,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="56" zoomScaleNormal="25" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3279,7 +3279,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3665,15 +3665,16 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="58" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="40.77734375" style="2" customWidth="1"/>
-    <col min="3" max="5" width="100.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="100.77734375" style="2" customWidth="1"/>
     <col min="6" max="9" width="40.77734375" style="2" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>

</xml_diff>